<commit_message>
All 2017 data K to Sap Plots
</commit_message>
<xml_diff>
--- a/Workflow.xlsx
+++ b/Workflow.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yliua\Desktop\MP.June\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D743CCA9-8C79-40A9-9F4F-7B6E3DA73146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38CD7CD-7289-43A8-88C8-4279667D3E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
     <sheet name="Expansion" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
   <si>
     <t>Notes</t>
   </si>
@@ -211,6 +212,36 @@
   </si>
   <si>
     <t>All 2017 data</t>
+  </si>
+  <si>
+    <t>https://github.com/AzuraLiu/MP.June/tree/main/Data/Processed/KtoSap</t>
+  </si>
+  <si>
+    <t>Sums</t>
+  </si>
+  <si>
+    <t>Daily, daytime, &amp; night sums</t>
+  </si>
+  <si>
+    <t>Not cleaned</t>
+  </si>
+  <si>
+    <t>Missing S3 March, S4 May, all Oct</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://github.com/AzuraLiu/MP.June/tree/main/Data/Processed/Sums/Raw</t>
+  </si>
+  <si>
+    <t>All 2017 Data</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>LBON17 missing Jan &amp; Feb; HCON4 missing Dec</t>
   </si>
 </sst>
 </file>
@@ -576,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51B019-8F72-4AFD-A957-B1F60307B36F}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,10 +914,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C6CE90-F53C-41AD-8EA1-92869D4DF72B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -935,6 +966,9 @@
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -943,10 +977,72 @@
       <c r="B4" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A6D1ECBE-355E-4CC6-847B-F15E90886560}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{F6B9241A-E338-4E89-B0A8-FF180EDF3643}"/>
+    <hyperlink ref="C6" r:id="rId3" xr:uid="{B1B99258-8151-4E87-857B-09BAF5A489A1}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{0A2C0173-F8CE-431A-86ED-BFBA82DABF03}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
July cleaning Inner probe cleaning
</commit_message>
<xml_diff>
--- a/Workflow.xlsx
+++ b/Workflow.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yliua\Desktop\MP.June\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38CD7CD-7289-43A8-88C8-4279667D3E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB2B0AF-A334-4D62-A14D-BEC3B45BDB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
     <sheet name="Expansion" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="80">
   <si>
     <t>Notes</t>
   </si>
@@ -238,10 +237,46 @@
     <t>All 2017 Data</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>LBON17 missing Jan &amp; Feb; HCON4 missing Dec</t>
+  </si>
+  <si>
+    <t>Statistical Analysis</t>
+  </si>
+  <si>
+    <t>N vs S</t>
+  </si>
+  <si>
+    <t>Unit conversion</t>
+  </si>
+  <si>
+    <t>Sapflux*Sapwood area=&gt;sapflow</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Interpolation</t>
+  </si>
+  <si>
+    <t>sapwood area analysis</t>
+  </si>
+  <si>
+    <t>found bug in code; previous analysis did not include inner probe</t>
+  </si>
+  <si>
+    <t>Data cleaning &amp; wrangling for inner probes, updated in previous files</t>
+  </si>
+  <si>
+    <t>plot (Q on S4.7.HAO6.1 &amp; 8.1)</t>
+  </si>
+  <si>
+    <t>cleaned</t>
+  </si>
+  <si>
+    <t>https://github.com/AzuraLiu/MP.June/tree/main/Data/Processed/Cleaned/Raw</t>
+  </si>
+  <si>
+    <t>Gap-filling</t>
   </si>
 </sst>
 </file>
@@ -265,7 +300,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +310,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -292,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -321,8 +362,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -605,17 +670,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51B019-8F72-4AFD-A957-B1F60307B36F}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="39" style="5" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="22.44140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" style="5" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
@@ -845,16 +910,30 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="18" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="A18" s="14"/>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>38</v>
@@ -864,12 +943,12 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="10"/>
-      <c r="B19" s="5" t="s">
-        <v>48</v>
+      <c r="A19" s="14"/>
+      <c r="B19" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>38</v>
@@ -878,24 +957,53 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="7" t="s">
+    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:5" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>27</v>
+      <c r="D21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A18:A20"/>
+  <mergeCells count="2">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{34DEF468-3F9D-45F7-9A73-DC2A75C17358}"/>
@@ -905,8 +1013,9 @@
     <hyperlink ref="C9" r:id="rId5" xr:uid="{6D73E7FC-2E08-4109-A997-9D286A22FF70}"/>
     <hyperlink ref="C14" r:id="rId6" xr:uid="{2739A07B-A8F0-4541-9B04-5A3CADF6D506}"/>
     <hyperlink ref="C16" r:id="rId7" xr:uid="{31431EEB-CC65-4311-AC4B-D732E413AFA4}"/>
-    <hyperlink ref="C19" r:id="rId8" xr:uid="{FDB8FD52-0655-4418-88BD-4501487858BD}"/>
-    <hyperlink ref="C20" r:id="rId9" xr:uid="{0D4C8CD9-A133-480A-AE2C-519B1DC81776}"/>
+    <hyperlink ref="C18" r:id="rId8" xr:uid="{FDB8FD52-0655-4418-88BD-4501487858BD}"/>
+    <hyperlink ref="C19" r:id="rId9" xr:uid="{0D4C8CD9-A133-480A-AE2C-519B1DC81776}"/>
+    <hyperlink ref="C21" r:id="rId10" xr:uid="{BE237272-6F1E-4668-AF35-AF10F261DC1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -914,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C6CE90-F53C-41AD-8EA1-92869D4DF72B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,34 +1124,87 @@
         <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:5" s="13" customFormat="1" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" s="5" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B8" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D13" s="1" t="s">
+      <c r="C8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" s="5" customFormat="1" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D15" s="1" t="s">
         <v>63</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{A6D1ECBE-355E-4CC6-847B-F15E90886560}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{F6B9241A-E338-4E89-B0A8-FF180EDF3643}"/>
     <hyperlink ref="C6" r:id="rId3" xr:uid="{B1B99258-8151-4E87-857B-09BAF5A489A1}"/>
     <hyperlink ref="C5" r:id="rId4" xr:uid="{0A2C0173-F8CE-431A-86ED-BFBA82DABF03}"/>
+    <hyperlink ref="C8" r:id="rId5" xr:uid="{6FF6C80D-3FDF-471A-9F1C-530DEA0E0B30}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{8713306F-CE71-4FB7-AEDB-D068DCBAF5C4}"/>
+    <hyperlink ref="C11" r:id="rId7" xr:uid="{A5BF830D-C8C3-4BDF-A135-C1566BEF6DB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
July Sapflow Plot level
</commit_message>
<xml_diff>
--- a/Workflow.xlsx
+++ b/Workflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yliua\Desktop\MP.June\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A546C5-C669-4BBC-A7EB-D995969CDE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E529A534-A80B-4C0C-A6B1-7554620C4324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2895" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="109">
   <si>
     <t>Notes</t>
   </si>
@@ -352,6 +352,18 @@
   </si>
   <si>
     <t>https://github.com/AzuraLiu/MP.June/tree/main/Data/Processed/Sapflow/Jun17/plots/byCrossSection</t>
+  </si>
+  <si>
+    <t>Plot Level Sapflow</t>
+  </si>
+  <si>
+    <t>Calculated sectional area sums across plots</t>
+  </si>
+  <si>
+    <t>July Sectional Sapflow (*sapflux/10000)</t>
+  </si>
+  <si>
+    <t>Graphs</t>
   </si>
 </sst>
 </file>
@@ -754,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51B019-8F72-4AFD-A957-B1F60307B36F}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1135,6 +1147,25 @@
       </c>
       <c r="C28" s="7" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B32" s="5" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Separated 4 blocks recalc sapflow
</commit_message>
<xml_diff>
--- a/Workflow.xlsx
+++ b/Workflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yliua\Desktop\MP.June\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335A92B8-3B7F-42B5-A139-23FE28F6DCCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D090972F-0DFF-4280-ADEB-57655EBC8172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2895" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="121">
   <si>
     <t>Notes</t>
   </si>
@@ -384,13 +384,22 @@
     <t>May</t>
   </si>
   <si>
-    <t>System 2 shut down, LBOS10, LBIS10 missing whole month</t>
-  </si>
-  <si>
     <t>Combined Metasheets</t>
   </si>
   <si>
     <t>May, Jun,  Jul,Aug</t>
+  </si>
+  <si>
+    <t>System 2 shut down, S3 LBOS10, LBIS10 missing whole month</t>
+  </si>
+  <si>
+    <t>Plot level sapflow</t>
+  </si>
+  <si>
+    <t>Separated 4 blocks (4*8)</t>
+  </si>
+  <si>
+    <t>Updated graphs</t>
   </si>
 </sst>
 </file>
@@ -793,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51B019-8F72-4AFD-A957-B1F60307B36F}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1147,25 +1156,38 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="E25" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="7"/>
+        <v>88</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="E26" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>84</v>
@@ -1173,62 +1195,67 @@
     </row>
     <row r="28" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>78</v>
       </c>
+      <c r="D28" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="E28" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A30" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="B30" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="7" t="s">
+    <row r="31" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B32" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="7" t="s">
+    </row>
+    <row r="33" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B33" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1250,11 +1277,13 @@
     <hyperlink ref="C22" r:id="rId11" xr:uid="{ACE6616C-8310-4D53-B467-75C2C122B9EB}"/>
     <hyperlink ref="C23" r:id="rId12" xr:uid="{4194C87A-A752-4C7F-BA15-BAD5AC403A7F}"/>
     <hyperlink ref="C24" r:id="rId13" xr:uid="{DA715786-006E-4C09-9F0A-7ACEEF54437C}"/>
-    <hyperlink ref="C27" r:id="rId14" xr:uid="{1D586E15-4E53-43F2-A086-3471FFCFD080}"/>
-    <hyperlink ref="C28" r:id="rId15" xr:uid="{71778FCA-24E3-4D73-99EE-B3BE5712C1E1}"/>
-    <hyperlink ref="C32" r:id="rId16" xr:uid="{FFBDFE5A-F8CC-477B-858C-67737A0E76B3}"/>
-    <hyperlink ref="C31" r:id="rId17" xr:uid="{1591CCC2-7440-4551-A3ED-435E5608CB92}"/>
-    <hyperlink ref="C30" r:id="rId18" xr:uid="{D6450849-BA59-4841-96DB-21439FBF2C20}"/>
+    <hyperlink ref="C26" r:id="rId14" xr:uid="{1D586E15-4E53-43F2-A086-3471FFCFD080}"/>
+    <hyperlink ref="C27" r:id="rId15" xr:uid="{71778FCA-24E3-4D73-99EE-B3BE5712C1E1}"/>
+    <hyperlink ref="C30" r:id="rId16" xr:uid="{FFBDFE5A-F8CC-477B-858C-67737A0E76B3}"/>
+    <hyperlink ref="C29" r:id="rId17" xr:uid="{1591CCC2-7440-4551-A3ED-435E5608CB92}"/>
+    <hyperlink ref="C28" r:id="rId18" xr:uid="{D6450849-BA59-4841-96DB-21439FBF2C20}"/>
+    <hyperlink ref="C32" r:id="rId19" xr:uid="{E4AF83F7-FEEF-489C-B498-D87DCDD3EE08}"/>
+    <hyperlink ref="C33" r:id="rId20" xr:uid="{98741C70-5CD6-48AA-9B63-8110AAA014C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1264,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C6CE90-F53C-41AD-8EA1-92869D4DF72B}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1517,18 +1546,18 @@
         <v>51</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>